<commit_message>
cfinished show inside clients
</commit_message>
<xml_diff>
--- a/app/python_logic/.PinUsuarios.xlsx
+++ b/app/python_logic/.PinUsuarios.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Cedula</t>
+  </si>
+  <si>
+    <t>A10</t>
   </si>
 </sst>
 </file>
@@ -374,15 +377,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1020810810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>